<commit_message>
spreadsheet changes (nozzle-cc calcs)
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB621FC-30A5-0F4B-91DC-0BBBA9967F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BDF10F-6B9B-E944-A792-00540CE078B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>SQRT( 4 * Exit Area / Pi)</t>
   </si>
   <si>
-    <t>Covergent Length + Divergrnt Length</t>
-  </si>
-  <si>
     <t>Chamber Area</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>(De / 2) * SIN(Nozzle Angles - 90 + 180) / SIN(Nozzle Angles)</t>
+  </si>
+  <si>
+    <t>Covergent Length + Divergent Length</t>
   </si>
 </sst>
 </file>
@@ -262,10 +262,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,18 +672,34 @@
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B7" s="6">
+        <v>5642.33</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -692,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -702,7 +718,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
@@ -712,14 +728,14 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="F2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -945,7 +961,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -953,7 +969,7 @@
         <v>39</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -961,7 +977,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -969,10 +985,10 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -980,7 +996,7 @@
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -988,7 +1004,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -996,7 +1012,7 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -1010,7 +1026,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1024,34 +1040,30 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C19:H19"/>
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="C23:H23"/>
     <mergeCell ref="C25:H25"/>
@@ -1068,9 +1080,13 @@
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
interfacing user flash space on stm32f4 and additions to control
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BDF10F-6B9B-E944-A792-00540CE078B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35EF7BF-7ACF-1E4E-8285-4DE204EAE590}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,11 +1061,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="K2:L2"/>
@@ -1080,13 +1082,11 @@
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
refactor of avionics docs with additions to firmware. Additions to nozzle/cc sheets
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35EF7BF-7ACF-1E4E-8285-4DE204EAE590}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5946C023-11C6-A845-94AA-DF8D7D485FF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Nozzle</t>
   </si>
@@ -188,6 +188,27 @@
   </si>
   <si>
     <t>Covergent Length + Divergent Length</t>
+  </si>
+  <si>
+    <t>Mixture Ratio</t>
+  </si>
+  <si>
+    <t>Optimum Expansion Ratio</t>
+  </si>
+  <si>
+    <t>k = Specific Heat Ratio</t>
+  </si>
+  <si>
+    <t>Po = Chamber Pressure</t>
+  </si>
+  <si>
+    <t>Pe = Exit Pressure</t>
+  </si>
+  <si>
+    <t>Chamber Characteristic Length (L*)</t>
+  </si>
+  <si>
+    <t>Chamber Volume / Throat Area</t>
   </si>
 </sst>
 </file>
@@ -250,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -266,6 +287,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -286,6 +310,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2348366</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>145918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{780C5038-6F68-5147-AACD-2DA5A99659FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2348366" y="3048000"/>
+          <a:ext cx="4230234" cy="1200018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -631,16 +704,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -693,6 +766,35 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
+    </row>
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="e">
+        <f xml:space="preserve"> Patm</f>
+        <v>#NAME?</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -701,15 +803,16 @@
     <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,6 +930,10 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -840,8 +947,10 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -853,8 +962,10 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -866,8 +977,13 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="6">
+        <f>Stats!B7 + 460</f>
+        <v>6102.33</v>
+      </c>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -875,7 +991,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -887,8 +1003,13 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" s="6">
+        <f>0.909*K19</f>
+        <v>5547.0179699999999</v>
+      </c>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -896,7 +1017,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -909,7 +1030,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -922,7 +1043,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -935,7 +1056,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -948,7 +1069,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1047,6 +1168,12 @@
       <c r="A43" t="s">
         <v>46</v>
       </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
       <c r="I43" t="s">
         <v>49</v>
       </c>
@@ -1055,19 +1182,42 @@
       <c r="A45" t="s">
         <v>47</v>
       </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
       <c r="I45" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
+  <mergeCells count="34">
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K21:L21"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="K2:L2"/>
@@ -1084,9 +1234,13 @@
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C13:H13"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
work on controller power assemblies(Li-ion docs additions + assembly casing additions)
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5946C023-11C6-A845-94AA-DF8D7D485FF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9056D3-C588-C74B-A24F-BE96B618F2A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Nozzle</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t>Chamber Volume / Throat Area</t>
+  </si>
+  <si>
+    <t>L* x Throat Area</t>
+  </si>
+  <si>
+    <t>Throat Diameter * 5</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
 </sst>
 </file>
@@ -283,13 +292,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -706,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,7 +725,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -727,7 +736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -741,7 +750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -749,7 +758,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -759,20 +768,25 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <v>300</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -811,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:H47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,7 +835,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
@@ -831,14 +845,14 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1029,6 +1043,11 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
+      <c r="K23" s="6">
+        <f>0.564*Stats!B9</f>
+        <v>169.2</v>
+      </c>
+      <c r="L23" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1042,6 +1061,11 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
+      <c r="K25" s="6">
+        <f>SQRT(4*K27/3.14)</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1055,6 +1079,11 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
+      <c r="K27" s="6">
+        <f>K13/K23 *SQRT(G4*K21)/(K9*K11)</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="6"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1068,6 +1097,11 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
+      <c r="K29" s="6">
+        <f>3.65*K27</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1084,8 +1118,13 @@
       <c r="I31" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K31" s="6">
+        <f>SQRT(4*K29/3.14)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1100,8 +1139,13 @@
       <c r="I33" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K33" s="6">
+        <f>K35+K37</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1119,8 +1163,10 @@
       <c r="I35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1135,12 +1181,16 @@
       <c r="I37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -1150,11 +1200,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="6"/>
+      <c r="C41" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -1164,21 +1216,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
       <c r="I43" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1192,7 +1244,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -1206,7 +1258,33 @@
       <c r="H47" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="42">
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K15:L15"/>
@@ -1220,27 +1298,9 @@
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C27:H27"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C13:H13"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update to AETS to include predefined comparison-based termination circumstances (unfinished)
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9056D3-C588-C74B-A24F-BE96B618F2A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AD31EA-A649-E246-A654-4E21220C1E48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
@@ -292,13 +292,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13:L13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,7 +835,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
@@ -845,14 +845,14 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="F2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1220,12 +1220,12 @@
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
       <c r="I43" t="s">
         <v>49</v>
       </c>
@@ -1259,32 +1259,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K15:L15"/>
@@ -1301,6 +1275,32 @@
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C13:H13"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
look over system telemetry/raw data and design equations
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AD31EA-A649-E246-A654-4E21220C1E48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126B7C9A-4A82-2840-811D-6348D3DA153A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Nozzle</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>Change</t>
+  </si>
+  <si>
+    <t>Gass Compressor capacity/Inlet flow</t>
+  </si>
+  <si>
+    <t>Isp = F / mass flow * gravity constant</t>
+  </si>
+  <si>
+    <t>&lt;- Change</t>
   </si>
 </sst>
 </file>
@@ -292,13 +301,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -713,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +734,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -736,7 +745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -750,15 +759,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <f>B1/(B27*9.80665)</f>
+        <v>187.6277831879388</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="E5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -768,7 +786,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -781,27 +799,27 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>58</v>
       </c>
@@ -810,11 +828,23 @@
         <v>#NAME?</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27">
+        <v>12.5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -825,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,7 +865,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
@@ -845,14 +875,14 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1220,12 +1250,12 @@
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
       <c r="I43" t="s">
         <v>49</v>
       </c>
@@ -1259,6 +1289,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K15:L15"/>
@@ -1275,32 +1331,6 @@
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C13:H13"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
ecu firmware changes and additional design docs
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126B7C9A-4A82-2840-811D-6348D3DA153A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63714248-86F6-A244-B6B9-F52E928A0148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
     <sheet name="Description" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -724,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,6 +804,9 @@
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -840,11 +844,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:H5"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -855,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13:L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,7 +980,8 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="K13" s="6">
-        <v>0</v>
+        <f>Stats!B1/Stats!B5</f>
+        <v>122.583125</v>
       </c>
       <c r="L13" s="6"/>
     </row>
@@ -991,7 +997,10 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="K15" s="6" t="e">
+        <f>(K13/Stats!B11)+1</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L15" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1006,7 +1015,10 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="K17" s="6" t="e">
+        <f>K13-K15</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L17" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1093,7 +1105,7 @@
       <c r="H25" s="6"/>
       <c r="K25" s="6">
         <f>SQRT(4*K27/3.14)</f>
-        <v>0</v>
+        <v>3.7870846269500515</v>
       </c>
       <c r="L25" s="6"/>
     </row>
@@ -1110,8 +1122,8 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="K27" s="6">
-        <f>K13/K23 *SQRT(G4*K21)/(K9*K11)</f>
-        <v>0</v>
+        <f>K13/K23 *SQRT(K4*K21)/(K9*K11)</f>
+        <v>11.258477827769909</v>
       </c>
       <c r="L27" s="6"/>
     </row>
@@ -1129,7 +1141,7 @@
       <c r="H29" s="6"/>
       <c r="K29" s="6">
         <f>3.65*K27</f>
-        <v>0</v>
+        <v>41.093444071360167</v>
       </c>
       <c r="L29" s="6"/>
     </row>
@@ -1150,7 +1162,7 @@
       </c>
       <c r="K31" s="6">
         <f>SQRT(4*K29/3.14)</f>
-        <v>0</v>
+        <v>7.2352150207604167</v>
       </c>
       <c r="L31" s="6"/>
     </row>

</xml_diff>

<commit_message>
written unit-tests for some ecu firmware modules and adiitions to design docs
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63714248-86F6-A244-B6B9-F52E928A0148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABBF3AF-F8EB-9B46-BAAC-028629F877A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
     <sheet name="Description" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -182,9 +181,6 @@
     <t>in^3</t>
   </si>
   <si>
-    <t>(Dt / 2) * SIN(RADIANS(a - 90 + 180)) / SIN(RADIANS(a)</t>
-  </si>
-  <si>
     <t>(De / 2) * SIN(Nozzle Angles - 90 + 180) / SIN(Nozzle Angles)</t>
   </si>
   <si>
@@ -228,6 +224,9 @@
   </si>
   <si>
     <t>&lt;- Change</t>
+  </si>
+  <si>
+    <t>(Dt / 2) * SIN(RADIANS(throat radius - 90 + 180)) / SIN(RADIANS(throat radius)</t>
   </si>
 </sst>
 </file>
@@ -302,13 +301,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -725,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,7 +770,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -797,12 +796,12 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -810,22 +809,22 @@
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" t="e">
         <f xml:space="preserve"> Patm</f>
@@ -834,13 +833,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27">
         <v>12.5</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -860,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,7 +869,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
@@ -880,14 +879,14 @@
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="F2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1171,7 +1170,7 @@
         <v>39</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1181,9 +1180,9 @@
       <c r="I33" t="s">
         <v>49</v>
       </c>
-      <c r="K33" s="6">
+      <c r="K33" s="6" t="e">
         <f>K35+K37</f>
-        <v>0</v>
+        <v>#NAME?</v>
       </c>
       <c r="L33" s="6"/>
     </row>
@@ -1195,7 +1194,7 @@
         <v>48</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1205,7 +1204,10 @@
       <c r="I35" t="s">
         <v>49</v>
       </c>
-      <c r="K35" s="6"/>
+      <c r="K35" s="6" t="e">
+        <f>(K25/2)*SI</f>
+        <v>#NAME?</v>
+      </c>
       <c r="L35" s="6"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -1213,7 +1215,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1231,7 +1233,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1241,13 +1243,15 @@
       <c r="I39" t="s">
         <v>50</v>
       </c>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1257,17 +1261,19 @@
       <c r="I41" t="s">
         <v>49</v>
       </c>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
       <c r="I43" t="s">
         <v>49</v>
       </c>
@@ -1288,45 +1294,27 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
+      <c r="K47" s="6">
+        <f>K39/K27</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="E2:F2"/>
+  <mergeCells count="45">
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K41:L41"/>
     <mergeCell ref="C47:H47"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K15:L15"/>
@@ -1343,6 +1331,32 @@
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C13:H13"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
changes to ecu firmware - mostly
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59FDE85-4C86-4D49-9FF6-B3420A000D63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC8E692-B982-2545-8CB1-56A6855F089F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
@@ -151,9 +151,6 @@
     <t>3.65 * Throat Area</t>
   </si>
   <si>
-    <t>SQRT( 4 * Exit Area / Pi)</t>
-  </si>
-  <si>
     <t>Chamber Area</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>!!</t>
+  </si>
+  <si>
+    <t>SQRT(4 * Exit Area / Pi)</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -345,11 +350,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +765,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1">
         <v>11240</v>
@@ -785,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
@@ -804,72 +804,72 @@
     </row>
     <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="7">
+        <v>65</v>
+      </c>
+      <c r="B5" s="9">
         <f>B1/(B27*9.80665)</f>
         <v>91.692881870975313</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="7">
+        <v>64</v>
+      </c>
+      <c r="B7" s="9">
         <v>5642.33</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="7">
+        <v>63</v>
+      </c>
+      <c r="B9" s="9">
         <v>100</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="7">
+        <v>67</v>
+      </c>
+      <c r="B11" s="9">
         <v>1.3</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" t="e">
         <f xml:space="preserve"> Patm</f>
@@ -877,17 +877,17 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>57</v>
+      <c r="A27" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="B27">
         <v>12.5</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -895,24 +895,24 @@
         <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
         <v>70</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>71</v>
-      </c>
-      <c r="C30" t="s">
-        <v>72</v>
       </c>
       <c r="D30">
         <v>14.6959</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:H13"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,24 +943,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="F2" s="11"/>
+      <c r="K2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -971,146 +971,146 @@
         <v>3</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="K4" s="7">
+      <c r="K4" s="9">
         <v>65</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="K9" s="7">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="K9" s="9">
         <v>1.2</v>
       </c>
-      <c r="L9" s="7"/>
+      <c r="L9" s="9"/>
     </row>
     <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="K11" s="7">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="K11" s="9">
         <v>32.200000000000003</v>
       </c>
-      <c r="L11" s="7"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="K13" s="7">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="K13" s="9">
         <f>Stats!B1/Stats!B5</f>
         <v>122.583125</v>
       </c>
-      <c r="L13" s="7"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="K15" s="7">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="K15" s="9">
         <f>(K13/Stats!B11)+1</f>
         <v>95.294711538461527</v>
       </c>
-      <c r="L15" s="7"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="K17" s="7">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="K17" s="9">
         <f>K13-K15</f>
         <v>27.288413461538468</v>
       </c>
-      <c r="L17" s="7"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="K19" s="7">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="K19" s="9">
         <f>Stats!B7 + 460</f>
         <v>6102.33</v>
       </c>
-      <c r="L19" s="7"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
@@ -1124,19 +1124,19 @@
       <c r="A21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="K21" s="7">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="K21" s="9">
         <f>0.909*K19</f>
         <v>5547.0179699999999</v>
       </c>
-      <c r="L21" s="7"/>
+      <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C22" s="4"/>
@@ -1150,94 +1150,94 @@
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="K23" s="7">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="K23" s="9">
         <f>0.564*Stats!B9</f>
         <v>56.399999999999991</v>
       </c>
-      <c r="L23" s="7"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="K25" s="7">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="K25" s="9">
         <f>SQRT(4*K27/3.14)</f>
         <v>6.5594229864405174</v>
       </c>
-      <c r="L25" s="7"/>
+      <c r="L25" s="9"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="K27" s="7">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="K27" s="9">
         <f>K13/K23 *SQRT(K4*K21)/(K9*K11)</f>
         <v>33.775433483309726</v>
       </c>
-      <c r="L27" s="7"/>
+      <c r="L27" s="9"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="K29" s="7">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="K29" s="9">
         <f>3.65*K27</f>
         <v>123.2803322140805</v>
       </c>
-      <c r="L29" s="7"/>
+      <c r="L29" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="C31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
       <c r="I31" t="s">
-        <v>45</v>
-      </c>
-      <c r="K31" s="7">
-        <f>SQRT(4*K29/3.14)</f>
+        <v>44</v>
+      </c>
+      <c r="K31" s="9">
+        <f>SQRT( 4* K29/3.14)</f>
         <v>12.531760019642551</v>
       </c>
-      <c r="L31" s="7"/>
+      <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C32" s="6"/>
@@ -1251,23 +1251,23 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="K33" s="7">
+        <v>68</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="K33" s="9">
         <f>2 / (K9-1)*(((Stats!B9/Stats!D30)^(Description!K9-1/Description!K9))-1)</f>
         <v>10.20046644155758</v>
       </c>
-      <c r="L33" s="7"/>
-      <c r="M33" s="12" t="s">
-        <v>74</v>
+      <c r="L33" s="9"/>
+      <c r="M33" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -1282,102 +1282,102 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="C35" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
       <c r="I35" t="s">
-        <v>45</v>
-      </c>
-      <c r="K35" s="7" t="e">
+        <v>44</v>
+      </c>
+      <c r="K35" s="9" t="e">
         <f>K37+K39</f>
         <v>#NAME?</v>
       </c>
-      <c r="L35" s="7"/>
+      <c r="L35" s="9"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" t="s">
-        <v>45</v>
-      </c>
-      <c r="K37" s="7" t="e">
+      <c r="K37" s="9" t="e">
         <f>(K25/2)*SI</f>
         <v>#NAME?</v>
       </c>
-      <c r="L37" s="7"/>
+      <c r="L37" s="9"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="C39" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
       <c r="I39" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
+      <c r="C41" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
       <c r="I41" t="s">
-        <v>46</v>
-      </c>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
       <c r="I43" t="s">
-        <v>45</v>
-      </c>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
@@ -1386,43 +1386,74 @@
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
       <c r="I45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
       <c r="I47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="K49" s="7">
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="K49" s="9">
         <f>K41/K27</f>
         <v>0</v>
       </c>
-      <c r="L49" s="7"/>
+      <c r="L49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="K49:L49"/>
     <mergeCell ref="K41:L41"/>
     <mergeCell ref="K43:L43"/>
@@ -1439,37 +1470,6 @@
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C37:H37"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K33:L33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
firmware and design changes
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48D2433-55EB-824C-8104-2C39D2BA3EAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BDED4D-5C23-B24B-932B-75F401BCF6DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="2" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="2" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>Gas Constant (R)</t>
   </si>
@@ -129,13 +129,7 @@
     <t>Exit Diameter (De)</t>
   </si>
   <si>
-    <t>Nozzle Length (Lnozzle)</t>
-  </si>
-  <si>
-    <t>Convergent Length (Lconvergent)</t>
-  </si>
-  <si>
-    <t>Divergent Length (Ldivergent)</t>
+    <t>Chamber Volume (Vc)</t>
   </si>
   <si>
     <t>Chamber Diameter (Dc)</t>
@@ -147,34 +141,22 @@
     <t>Chamber Length</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>in</t>
   </si>
   <si>
-    <t>(De / 2) * SIN(Nozzle Angles - 90 + 180) / SIN(Nozzle Angles)</t>
-  </si>
-  <si>
-    <t>Covergent Length + Divergent Length</t>
-  </si>
-  <si>
     <t>Optimum Expansion Ratio</t>
   </si>
   <si>
     <t>Chamber Characteristic Length (L*)</t>
   </si>
   <si>
-    <t>Chamber Volume / Throat Area</t>
+    <t>L* x Throat Area</t>
   </si>
   <si>
     <t>Change</t>
   </si>
   <si>
     <t>Isp = F / mass flow * gravity constant</t>
-  </si>
-  <si>
-    <t>(Dt / 2) * SIN(RADIANS(throat radius - 90 + 180)) / SIN(RADIANS(throat radius)</t>
   </si>
   <si>
     <t>50kn</t>
@@ -298,13 +280,34 @@
   </si>
   <si>
     <t>Inlet flow</t>
+  </si>
+  <si>
+    <t>Nozzle Length  (the percentage length of a 15 degree conical nozzle)</t>
+  </si>
+  <si>
+    <t>Bell Length</t>
+  </si>
+  <si>
+    <t>Conical Nozzle Angle</t>
+  </si>
+  <si>
+    <t>(Exit Radius - Throat Radius) / np.tan(np.deg2rad(Conical Nozzle angle)) * bell_length</t>
+  </si>
+  <si>
+    <t>Exit Radius (Re)</t>
+  </si>
+  <si>
+    <t>Exit Diameter / 2</t>
+  </si>
+  <si>
+    <t>Contraction area ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +344,13 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -391,6 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,12 +828,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>11240</v>
@@ -831,7 +842,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -839,7 +850,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <v>50</v>
@@ -867,7 +878,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B9" s="6">
         <f>B3/(B5*9.80665)</f>
@@ -876,7 +887,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -887,7 +898,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B11" s="6">
         <v>5642.33</v>
@@ -900,7 +911,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B13" s="6">
         <v>100</v>
@@ -908,7 +919,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -916,7 +927,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B15" s="6">
         <v>1.3</v>
@@ -928,20 +939,25 @@
       <c r="A16" s="11"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
+      <c r="A17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="6">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="A18" s="11"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
+      <c r="A19" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>0</v>
-      </c>
+      <c r="A20" s="11"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>2</v>
@@ -953,7 +969,9 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12" t="s">
+        <v>0</v>
+      </c>
       <c r="C21" s="6" t="s">
         <v>3</v>
       </c>
@@ -995,11 +1013,9 @@
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>76</v>
-      </c>
+      <c r="A25" s="11"/>
       <c r="C25" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1012,12 +1028,12 @@
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
+      <c r="A26" s="11" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>72</v>
-      </c>
+      <c r="A27" s="11"/>
       <c r="C27" s="6" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1048,9 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
+      <c r="A28" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -1043,11 +1061,9 @@
       <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>73</v>
-      </c>
+      <c r="A29" s="13"/>
       <c r="C29" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1060,16 +1076,16 @@
       </c>
       <c r="L29" s="6"/>
       <c r="M29" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
+      <c r="A30" s="13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A31" s="11"/>
       <c r="C31" s="6" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1100,9 @@
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
+      <c r="A32" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -1095,9 +1113,7 @@
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
-        <v>86</v>
-      </c>
+      <c r="A33" s="13"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -1107,25 +1123,33 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D35">
         <v>14.6959</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="C29:H29"/>
@@ -1154,7 +1178,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,7 +1190,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1310,10 +1334,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1336,28 +1360,23 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>45</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="K18" s="6" t="e">
-        <f>#REF!/#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1379,10 +1398,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1392,7 +1411,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M27" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.2">
@@ -1434,28 +1453,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A288A652-25F1-A940-BC3C-A6B5AB550EFC}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1509,7 +1528,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1527,7 +1546,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1535,7 +1554,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K11" s="6">
         <f>SQRT( 4* K9/3.14)</f>
@@ -1543,99 +1562,106 @@
       </c>
       <c r="L11" s="6"/>
     </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>33</v>
+      <c r="A13" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="6" t="e">
-        <f>K15+K17</f>
-        <v>#NAME?</v>
+      <c r="K13" s="6">
+        <f>K11/2</f>
+        <v>12.501526361487178</v>
       </c>
       <c r="L13" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="6" t="e">
-        <f>(K3/2)*SI</f>
-        <v>#NAME?</v>
+      <c r="K15" s="6">
+        <f>Properties!K18*Geometry!K7</f>
+        <v>0</v>
       </c>
       <c r="L15" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="6"/>
+      <c r="K17" s="6">
+        <f>K7*Constants!B17</f>
+        <v>672.25318724965871</v>
+      </c>
       <c r="L17" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="K19" s="6">
+        <f>SQRT(K17/3.14)</f>
+        <v>14.631929870511275</v>
+      </c>
       <c r="L19" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
       <c r="K21" s="6">
-        <f>SQRT(K19/3.14)</f>
-        <v>0</v>
+        <f xml:space="preserve"> 2*K19</f>
+        <v>29.26385974102255</v>
       </c>
       <c r="L21" s="6"/>
     </row>
@@ -1643,43 +1669,40 @@
       <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="6">
-        <f xml:space="preserve"> 2*K21</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="6"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>80</v>
+      <c r="K25" s="6">
+        <f>0.382*K3</f>
+        <v>2.4996544232009303</v>
+      </c>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1687,46 +1710,84 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="K27" s="6">
-        <f>0.382*K3</f>
-        <v>2.4996544232009303</v>
-      </c>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="K29" s="6">
         <f>1.5*K3</f>
         <v>9.8153969497418725</v>
       </c>
-      <c r="L29" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="K32" s="6">
+        <f>(K13-K3)/TAN(RADIANS(K36))*K34</f>
+        <v>17.788233182375734</v>
+      </c>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="K34" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="6">
+        <v>15</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="K36" s="6">
+        <v>15</v>
+      </c>
+      <c r="L36" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="K29:L29"/>
+  <mergeCells count="31">
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="K19:L19"/>
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="C23:H23"/>
-    <mergeCell ref="K23:L23"/>
     <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="K19:L19"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="C11:H11"/>

</xml_diff>

<commit_message>
tiny changes everywhere - can it get any tinier?
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BDED4D-5C23-B24B-932B-75F401BCF6DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CD269E-551E-7048-AFBB-42E0F409371B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="2" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>Gas Constant (R)</t>
   </si>
@@ -301,6 +301,18 @@
   </si>
   <si>
     <t>Contraction area ratio</t>
+  </si>
+  <si>
+    <t>Nozzle Convergent Length</t>
+  </si>
+  <si>
+    <t>Nozzle Divergent Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Dt / 2) * SIN(RADIANS(throat radius - 90 + 180)) / SIN(RADIANS(throat radius)					</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(De / 2) * SIN(Nozzle Angles - 90 + 180) / SIN(Nozzle Angles)					</t>
   </si>
 </sst>
 </file>
@@ -1453,10 +1465,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A288A652-25F1-A940-BC3C-A6B5AB550EFC}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:H23"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="84" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1767,8 +1779,48 @@
       </c>
       <c r="L36" s="6"/>
     </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="K38" s="6">
+        <f>(K5/2)*SIN(RADIANS(K3-90+180))/SIN(RADIANS(K3))</f>
+        <v>57.046453680331837</v>
+      </c>
+      <c r="L38" s="6"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="K40" s="6">
+        <f>K11/2*SIN(K36-90+180)/SIN(K36)</f>
+        <v>-18.658156715595034</v>
+      </c>
+      <c r="L40" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="35">
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K40:L40"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="C32:H32"/>

</xml_diff>

<commit_message>
unit tests for PTAM + injector stuff
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B17532-0DED-A449-BAA4-B32933BBC588}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7985954D-5795-B94B-A517-3AC7E0111B97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="13940" yWindow="500" windowWidth="14280" windowHeight="16300" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Geometry" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>M = Gas Molecular Weight (Combustion of gaseous/hydrocarbon fuel)  = 24</t>
   </si>
@@ -45,9 +46,6 @@
     <t>Calculations</t>
   </si>
   <si>
-    <t>lbf</t>
-  </si>
-  <si>
     <t>Propellants:</t>
   </si>
   <si>
@@ -102,9 +100,6 @@
     <t>Throat Area (At)</t>
   </si>
   <si>
-    <t>(wt/ Pt) * SQRT((R * Tt) / (y * g)</t>
-  </si>
-  <si>
     <t>Earths Gravitation (g)</t>
   </si>
   <si>
@@ -126,9 +121,6 @@
     <t>Chamber Length</t>
   </si>
   <si>
-    <t>in</t>
-  </si>
-  <si>
     <t>Optimum Expansion Ratio</t>
   </si>
   <si>
@@ -141,12 +133,6 @@
     <t>Change</t>
   </si>
   <si>
-    <t>Isp = F / mass flow * gravity constant</t>
-  </si>
-  <si>
-    <t>50kn</t>
-  </si>
-  <si>
     <t>Chamber Pressure (Pc)</t>
   </si>
   <si>
@@ -162,12 +148,6 @@
     <t xml:space="preserve">Mixture Ratio (r) </t>
   </si>
   <si>
-    <t xml:space="preserve">Exit Velocity </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 101.3 kPa</t>
-  </si>
-  <si>
     <t>2 / (SHR - 1) * [((Chamber Pressure / Atm Pressure) ^ (SHR - 1 / SHR)) - 1]</t>
   </si>
   <si>
@@ -177,15 +157,9 @@
     <t>SQRT(4 * Exit Area / Pi)</t>
   </si>
   <si>
-    <t>2 * Chamber Radius</t>
-  </si>
-  <si>
     <t>Chamber Radius (Rc)</t>
   </si>
   <si>
-    <t>sqrt(Chamber Area / pi)</t>
-  </si>
-  <si>
     <t>Chamber Area (Ac)</t>
   </si>
   <si>
@@ -196,9 +170,6 @@
   </si>
   <si>
     <t>sqrt(Throat Area / PI)</t>
-  </si>
-  <si>
-    <t>Characteristic Velocity</t>
   </si>
   <si>
     <t xml:space="preserve"> sqrt(gamma * Rspecific * Tc) / (
@@ -221,9 +192,6 @@
     <t>Universal gas constant (R_bar)</t>
   </si>
   <si>
-    <t>Geometry (Imperial Units)</t>
-  </si>
-  <si>
     <t>Rn - radius of circular entrance region for parabolic approximation (rao)
         i.e. region leaving the throat</t>
   </si>
@@ -325,13 +293,52 @@
   </si>
   <si>
     <t>Gas Molecular Weight</t>
+  </si>
+  <si>
+    <t>Exit Velocity (Ve)</t>
+  </si>
+  <si>
+    <t>Characteristic Velocity (c*)</t>
+  </si>
+  <si>
+    <t>Thrust Coefficient (Cf)</t>
+  </si>
+  <si>
+    <t>(mdot * Specific Impulse ) / Chamber Pressure * Thrust Coefficient</t>
+  </si>
+  <si>
+    <t>Chamber Volume / ( 1.1 * Chamber Area)</t>
+  </si>
+  <si>
+    <t>sqrt(4 * Chamber Area / pi)</t>
+  </si>
+  <si>
+    <t>Chamber Diameter / 2</t>
+  </si>
+  <si>
+    <t>kpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isp = Characteristic Velocity * Thrust Coefficient / gravity </t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>125 atm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -377,6 +384,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FFC9D1D9"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="2"/>
@@ -386,6 +399,12 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -409,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -427,6 +446,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,8 +462,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,6 +566,50 @@
         <a:xfrm>
           <a:off x="14744700" y="139699"/>
           <a:ext cx="4940300" cy="3201654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>37020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1879600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{374FEC29-288B-594E-AAE4-996DF9486901}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3314700" y="4913820"/>
+          <a:ext cx="5981700" cy="977901"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -856,72 +921,72 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="23" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>94</v>
+      <c r="A1" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>84</v>
+      <c r="A3" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>85</v>
+      <c r="A4" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>86</v>
+      <c r="A5" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>87</v>
+      <c r="A6" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>88</v>
+      <c r="A7" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>89</v>
+      <c r="A8" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>90</v>
+      <c r="A9" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>91</v>
+      <c r="A10" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>92</v>
+      <c r="A11" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="B11" s="7"/>
     </row>
@@ -935,7 +1000,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,239 +1009,245 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3">
-        <v>11240</v>
+        <v>10000</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="11">
-        <f>B3/(B5*9.80665)</f>
-        <v>22.923220467743828</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="B9" s="15">
+        <f>Properties!K20*Properties!K25/Constants!K29</f>
+        <v>244.72375127421</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="11">
+        <v>35</v>
+      </c>
+      <c r="B11" s="15">
         <v>5642.33</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="11">
-        <v>5000</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="B13" s="15">
+        <v>12665.6</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
       <c r="E13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="11">
-        <v>1.3</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="B15" s="15">
+        <v>1.31</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="11">
+        <v>68</v>
+      </c>
+      <c r="B17" s="15">
         <v>5</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="K20" s="11">
-        <v>65</v>
-      </c>
-      <c r="L20" s="11"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="K21" s="15">
+        <v>23.1</v>
+      </c>
+      <c r="L21" s="15"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="K23" s="11">
+        <v>52</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="K23" s="15">
         <v>8314</v>
       </c>
-      <c r="L23" s="11"/>
+      <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="K25" s="11">
-        <v>1.2</v>
-      </c>
-      <c r="L25" s="11"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="K25" s="15">
+        <v>1.1850000000000001</v>
+      </c>
+      <c r="L25" s="15"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="K27" s="11">
+        <v>49</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="K27" s="15">
         <f>K23/24</f>
         <v>346.41666666666669</v>
       </c>
-      <c r="L27" s="11"/>
+      <c r="L27" s="15"/>
       <c r="M27" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="K29" s="11">
+        <v>23</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="K29" s="15">
         <v>9.81</v>
       </c>
-      <c r="L29" s="11"/>
+      <c r="L29" s="15"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
@@ -1191,19 +1262,25 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L31" s="11"/>
+        <v>59</v>
+      </c>
+      <c r="K31" s="15">
+        <v>101.3</v>
+      </c>
+      <c r="L31" s="15"/>
+      <c r="M31" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="K27:L27"/>
     <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K21:L21"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B9:D9"/>
@@ -1218,8 +1295,6 @@
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="K25:L25"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="K27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1228,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:H10"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1241,99 +1316,102 @@
     <col min="8" max="8" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="E2" s="13" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="F2" s="17"/>
+      <c r="K2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="13"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="17"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="K4" s="15">
+        <f>Constants!B3/Constants!B9</f>
+        <v>40.862400759765734</v>
+      </c>
+      <c r="L4" s="15"/>
+      <c r="M4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="K4" s="11">
-        <f>Constants!B3/Constants!B9</f>
-        <v>490.33249999999998</v>
-      </c>
-      <c r="L4" s="11"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="K6" s="15">
+        <f>(K4/Constants!B15)+1</f>
+        <v>32.192672335699029</v>
+      </c>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="K8" s="15">
+        <f>K4-K6</f>
+        <v>8.6697284240667045</v>
+      </c>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="K6" s="11">
-        <f>(K4/Constants!B15)+1</f>
-        <v>378.17884615384611</v>
-      </c>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="K8" s="11">
-        <f>K4-K6</f>
-        <v>112.15365384615387</v>
-      </c>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="K10" s="11">
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="K10" s="15">
         <f>Constants!B11 + 460</f>
         <v>6102.33</v>
       </c>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1341,25 +1419,25 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="K12" s="11">
+        <v>19</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="K12" s="15">
         <f>0.909*K10</f>
         <v>5547.0179699999999</v>
       </c>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1367,43 +1445,43 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="K14" s="11">
+        <v>20</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="K14" s="15">
         <f>0.564*Constants!B13</f>
-        <v>2819.9999999999995</v>
-      </c>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>7143.3983999999991</v>
+      </c>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="K16" s="11" t="e">
+        <v>87</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="K16" s="15" t="e">
         <f>2 / (#REF!-1)*(((Constants!B13/Constants!D32)^(Properties!#REF!-1/Properties!#REF!))-1)</f>
         <v>#REF!</v>
       </c>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1411,75 +1489,93 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="K20" s="16">
+        <v>1535</v>
+      </c>
+      <c r="L20" s="15"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="16">
+        <v>2.5982911572999998</v>
+      </c>
+      <c r="O20" s="15"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="K20" s="12">
-        <v>2.5982911572999998</v>
-      </c>
-      <c r="L20" s="11"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="M23">
+        <v>1807.1590000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="K25" s="15">
+        <v>1.5640000000000001</v>
+      </c>
+      <c r="L25" s="15"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M27" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N35">
         <f>K20*K4/Constants!B13</f>
-        <v>0.25480531977736043</v>
+        <v>4.9522948116346956</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K12:L12"/>
+  <mergeCells count="25">
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C4:H4"/>
@@ -1489,6 +1585,14 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K8:L8"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K12:L12"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="C20:H21"/>
     <mergeCell ref="C23:H23"/>
@@ -1508,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A288A652-25F1-A940-BC3C-A6B5AB550EFC}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40:L40"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1519,101 +1623,98 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="K3" s="11">
+        <v>45</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="K3" s="15">
         <f>SQRT(Geometry!K7/3.14)</f>
-        <v>2.5535562140378878</v>
-      </c>
-      <c r="L3" s="11"/>
+        <v>0.62710558155261797</v>
+      </c>
+      <c r="L3" s="15"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="K5" s="11">
+        <v>21</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="K5" s="15">
         <f>SQRT(4*K7/3.14)</f>
-        <v>5.1071124280757756</v>
-      </c>
-      <c r="L5" s="11"/>
+        <v>1.2542111631052359</v>
+      </c>
+      <c r="L5" s="15"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="K7" s="11">
-        <f>Properties!K4/Properties!K14 *SQRT(Constants!K27*Properties!K12)/(Constants!K25*Constants!K29)</f>
-        <v>20.474838922109743</v>
-      </c>
-      <c r="L7" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="K7" s="15">
+        <f>Properties!K4*Constants!B9/Constants!B13*Properties!K25</f>
+        <v>1.2348408287013644</v>
+      </c>
+      <c r="L7" s="15"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="K9" s="11">
+        <v>24</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="K9" s="15">
         <f>3.65*K7</f>
-        <v>74.733162065700554</v>
-      </c>
-      <c r="L9" s="11"/>
+        <v>4.50716902475998</v>
+      </c>
+      <c r="L9" s="15"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="11">
+        <v>25</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="K11" s="15">
         <f>SQRT( 4* K9/3.14)</f>
-        <v>9.757124593776183</v>
-      </c>
-      <c r="L11" s="11"/>
+        <v>2.3961670626337659</v>
+      </c>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
@@ -1627,260 +1728,238 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="K13" s="11">
+        <v>66</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="K13" s="15">
         <f>K11/2</f>
-        <v>4.8785622968880915</v>
-      </c>
-      <c r="L13" s="11"/>
+        <v>1.1980835313168829</v>
+      </c>
+      <c r="L13" s="15"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="K15" s="11">
+        <v>26</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="K15" s="15">
         <f>Properties!K18*Geometry!K7</f>
         <v>0</v>
       </c>
-      <c r="L15" s="11"/>
+      <c r="L15" s="15"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="K17" s="11">
+        <v>43</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="K17" s="15">
         <f>K7*Constants!B17</f>
-        <v>102.37419461054871</v>
-      </c>
-      <c r="L17" s="11"/>
+        <v>6.174204143506822</v>
+      </c>
+      <c r="L17" s="15"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="K19" s="11">
-        <f>SQRT(K17/3.14)</f>
-        <v>5.70992527895572</v>
-      </c>
-      <c r="L19" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="K19" s="15">
+        <f>K21/2</f>
+        <v>1.4018958157520383</v>
+      </c>
+      <c r="L19" s="15"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="11">
-        <f xml:space="preserve"> 2*K19</f>
-        <v>11.41985055791144</v>
-      </c>
-      <c r="L21" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="K21" s="15">
+        <f>SQRT(4*K17/3.14159)</f>
+        <v>2.8037916315040765</v>
+      </c>
+      <c r="L21" s="15"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" t="s">
-        <v>32</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="K23" s="15">
+        <f>K15/(1.1*K17)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="15"/>
     </row>
     <row r="25" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="K25" s="11">
+        <v>53</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="K25" s="15">
         <f>0.382*K3</f>
-        <v>0.97545847376247319</v>
-      </c>
-      <c r="L25" s="11"/>
+        <v>0.23955433215310007</v>
+      </c>
+      <c r="L25" s="15"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="K27" s="11">
+        <v>55</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="K27" s="15">
         <f>1.5*K3</f>
-        <v>3.8303343210568315</v>
-      </c>
-      <c r="L27" s="11"/>
+        <v>0.94065837232892702</v>
+      </c>
+      <c r="L27" s="15"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="K32" s="11">
+        <v>62</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="K32" s="15">
         <f>(K13-K3)/TAN(RADIANS(K36))*K34</f>
-        <v>6.9416326632829239</v>
-      </c>
-      <c r="L32" s="11"/>
+        <v>1.7047349748173977</v>
+      </c>
+      <c r="L32" s="15"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="11">
+        <v>63</v>
+      </c>
+      <c r="C34" s="15">
         <v>0.8</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="K34" s="11">
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="K34" s="15">
         <v>0.8</v>
       </c>
-      <c r="L34" s="11"/>
+      <c r="L34" s="15"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="11">
+        <v>64</v>
+      </c>
+      <c r="C36" s="15">
         <v>15</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="K36" s="11">
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="K36" s="15">
         <v>15</v>
       </c>
-      <c r="L36" s="11"/>
+      <c r="L36" s="15"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="K38" s="11">
+        <v>69</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="K38" s="15">
         <f>(K5/2)*SIN(RADIANS(K3-90+180))/SIN(RADIANS(K3))</f>
-        <v>57.25783888858431</v>
-      </c>
-      <c r="L38" s="11"/>
+        <v>57.293491592666015</v>
+      </c>
+      <c r="L38" s="15"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="K40" s="11">
+        <v>70</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="K40" s="15">
         <f>K11/2*SIN(K36-90+180)/SIN(K36)</f>
-        <v>-7.2811093021846789</v>
-      </c>
-      <c r="L40" s="11"/>
+        <v>-1.7881040793985641</v>
+      </c>
+      <c r="L40" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C23:H23"/>
+  <mergeCells count="36">
     <mergeCell ref="C38:H38"/>
     <mergeCell ref="C40:H40"/>
     <mergeCell ref="K38:L38"/>
@@ -1893,6 +1972,30 @@
     <mergeCell ref="K34:L34"/>
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tiny changes everywhere - has anything even changed?
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7985954D-5795-B94B-A517-3AC7E0111B97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F04533-3788-5640-ABF6-85D243FE2B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="500" windowWidth="14280" windowHeight="16300" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="12920" yWindow="500" windowWidth="14280" windowHeight="16280" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="4" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t xml:space="preserve">Mixture Ratio (r) </t>
   </si>
   <si>
-    <t>2 / (SHR - 1) * [((Chamber Pressure / Atm Pressure) ^ (SHR - 1 / SHR)) - 1]</t>
-  </si>
-  <si>
     <t>!!</t>
   </si>
   <si>
@@ -208,12 +205,6 @@
     <t>Mach number at nozzle exit (Ma_exit)</t>
   </si>
   <si>
-    <t>SQRT(2 / (gamma - 1) * ((Chamber Pressure / ) ** ((gamma - 1) / gamma) - 1))</t>
-  </si>
-  <si>
-    <t>Ambient Pressure</t>
-  </si>
-  <si>
     <t>Constants</t>
   </si>
   <si>
@@ -332,6 +323,15 @@
   </si>
   <si>
     <t>125 atm</t>
+  </si>
+  <si>
+    <t>Ambient Pressure (Pa)</t>
+  </si>
+  <si>
+    <t>Ve = Me * sqrt (gam * R * Te)</t>
+  </si>
+  <si>
+    <t>sqrt(2 / (gamma - 1) * ((pc / pa) ** ((gamma - 1) / gamma) - 1))</t>
   </si>
 </sst>
 </file>
@@ -928,7 +928,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -938,55 +938,55 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B11" s="7"/>
     </row>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,7 +1011,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1022,7 +1022,7 @@
         <v>10000</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1030,7 +1030,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>50</v>
@@ -1065,12 +1065,12 @@
       </c>
       <c r="B9" s="15">
         <f>Properties!K20*Properties!K25/Constants!K29</f>
-        <v>244.72375127421</v>
+        <v>41.99143662814955</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -1085,10 +1085,13 @@
         <v>35</v>
       </c>
       <c r="B11" s="15">
-        <v>5642.33</v>
+        <v>3030</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
+      <c r="E11">
+        <v>5442.33</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1098,15 +1101,15 @@
         <v>34</v>
       </c>
       <c r="B13" s="15">
-        <v>12665.6</v>
+        <v>5000</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1127,7 +1130,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B17" s="15">
         <v>5</v>
@@ -1142,6 +1145,11 @@
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="K19" s="15">
+        <f>Geometry!K9/Geometry!K7</f>
+        <v>3.6499999999999995</v>
+      </c>
+      <c r="L19" s="15"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
@@ -1152,7 +1160,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -1173,10 +1181,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -1193,7 +1201,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>1</v>
@@ -1213,10 +1221,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -1229,7 +1237,7 @@
       </c>
       <c r="L27" s="15"/>
       <c r="M27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1237,7 +1245,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
@@ -1262,23 +1270,24 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="K31" s="15">
         <v>101.3</v>
       </c>
       <c r="L31" s="15"/>
       <c r="M31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K19:L19"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="B11:D11"/>
@@ -1303,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1318,7 +1327,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -1350,11 +1359,11 @@
       <c r="H4" s="15"/>
       <c r="K4" s="15">
         <f>Constants!B3/Constants!B9</f>
-        <v>40.862400759765734</v>
+        <v>238.14379318702231</v>
       </c>
       <c r="L4" s="15"/>
       <c r="M4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1371,7 +1380,7 @@
       <c r="H6" s="15"/>
       <c r="K6" s="15">
         <f>(K4/Constants!B15)+1</f>
-        <v>32.192672335699029</v>
+        <v>182.78915510459717</v>
       </c>
       <c r="L6" s="15"/>
     </row>
@@ -1389,7 +1398,7 @@
       <c r="H8" s="15"/>
       <c r="K8" s="15">
         <f>K4-K6</f>
-        <v>8.6697284240667045</v>
+        <v>55.35463808242514</v>
       </c>
       <c r="L8" s="15"/>
     </row>
@@ -1407,7 +1416,7 @@
       <c r="H10" s="15"/>
       <c r="K10" s="15">
         <f>Constants!B11 + 460</f>
-        <v>6102.33</v>
+        <v>3490</v>
       </c>
       <c r="L10" s="15"/>
     </row>
@@ -1433,7 +1442,7 @@
       <c r="H12" s="15"/>
       <c r="K12" s="15">
         <f>0.909*K10</f>
-        <v>5547.0179699999999</v>
+        <v>3172.4100000000003</v>
       </c>
       <c r="L12" s="15"/>
     </row>
@@ -1459,29 +1468,29 @@
       <c r="H14" s="15"/>
       <c r="K14" s="15">
         <f>0.564*Constants!B13</f>
-        <v>7143.3983999999991</v>
+        <v>2819.9999999999995</v>
       </c>
       <c r="L14" s="15"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="K16" s="15" t="e">
-        <f>2 / (#REF!-1)*(((Constants!B13/Constants!D32)^(Properties!#REF!-1/Properties!#REF!))-1)</f>
-        <v>#REF!</v>
+      <c r="K16" s="15">
+        <f>K23*SQRT(Constants!K25*Constants!K23)</f>
+        <v>62.978917667356583</v>
       </c>
       <c r="L16" s="15"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1489,7 +1498,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1502,12 +1511,12 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1515,16 +1524,22 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="K20" s="16">
-        <v>1535</v>
-      </c>
-      <c r="L20" s="15"/>
-      <c r="M20" s="14"/>
+        <v>263.38618498858511</v>
+      </c>
+      <c r="L20" s="16"/>
+      <c r="M20" s="14">
+        <f>SQRT(Constants!K29*Constants!K25*Constants!B11)/Constants!K25*SQRT(POWER(2/Constants!K25+1,Constants!K25+1/Constants!K25-1))</f>
+        <v>263.38618498858511</v>
+      </c>
       <c r="N20" s="16">
         <v>2.5982911572999998</v>
       </c>
       <c r="O20" s="15"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1532,25 +1547,30 @@
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
+      <c r="K23" s="15">
+        <f>SQRT(2/(Constants!K25-1)*POWER((Constants!B13/Constants!K31),((Constants!K25-1)/Constants!K25)-1))</f>
+        <v>0.63449909572023711</v>
+      </c>
+      <c r="L23" s="15"/>
       <c r="M23">
         <v>1807.1590000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -1562,20 +1582,28 @@
         <v>1.5640000000000001</v>
       </c>
       <c r="L25" s="15"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <f>0.985*SQRT((2*POWER(Constants!K25,2)/Constants!K25-1)*POWER(2/Constants!K25+1,Constants!K25+1/Constants!K25-1)*(1-POWER(Constants!K31/Constants!B13,Constants!K25-1/Constants!K25)+Constants!K19*(Constants!K31-Constants!K31/Constants!B13)))</f>
+        <v>36.900496921625056</v>
+      </c>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N35">
         <f>K20*K4/Constants!B13</f>
-        <v>4.9522948116346956</v>
+        <v>12.544757033248082</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="K23:L23"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C4:H4"/>
@@ -1612,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A288A652-25F1-A940-BC3C-A6B5AB550EFC}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1623,15 +1651,15 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -1640,7 +1668,7 @@
       <c r="H3" s="15"/>
       <c r="K3" s="15">
         <f>SQRT(Geometry!K7/3.14)</f>
-        <v>0.62710558155261797</v>
+        <v>0.99808734284582756</v>
       </c>
       <c r="L3" s="15"/>
     </row>
@@ -1658,7 +1686,7 @@
       <c r="H5" s="15"/>
       <c r="K5" s="15">
         <f>SQRT(4*K7/3.14)</f>
-        <v>1.2542111631052359</v>
+        <v>1.9961746856916551</v>
       </c>
       <c r="L5" s="15"/>
     </row>
@@ -1667,7 +1695,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -1676,7 +1704,7 @@
       <c r="H7" s="15"/>
       <c r="K7" s="15">
         <f>Properties!K4*Constants!B9/Constants!B13*Properties!K25</f>
-        <v>1.2348408287013644</v>
+        <v>3.1280000000000001</v>
       </c>
       <c r="L7" s="15"/>
     </row>
@@ -1694,7 +1722,7 @@
       <c r="H9" s="15"/>
       <c r="K9" s="15">
         <f>3.65*K7</f>
-        <v>4.50716902475998</v>
+        <v>11.417199999999999</v>
       </c>
       <c r="L9" s="15"/>
     </row>
@@ -1703,7 +1731,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -1712,7 +1740,7 @@
       <c r="H11" s="15"/>
       <c r="K11" s="15">
         <f>SQRT( 4* K9/3.14)</f>
-        <v>2.3961670626337659</v>
+        <v>3.8136863821840477</v>
       </c>
       <c r="L11" s="15"/>
     </row>
@@ -1728,10 +1756,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -1740,7 +1768,7 @@
       <c r="H13" s="15"/>
       <c r="K13" s="15">
         <f>K11/2</f>
-        <v>1.1980835313168829</v>
+        <v>1.9068431910920238</v>
       </c>
       <c r="L13" s="15"/>
     </row>
@@ -1764,10 +1792,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -1776,16 +1804,16 @@
       <c r="H17" s="15"/>
       <c r="K17" s="15">
         <f>K7*Constants!B17</f>
-        <v>6.174204143506822</v>
+        <v>15.64</v>
       </c>
       <c r="L17" s="15"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -1794,7 +1822,7 @@
       <c r="H19" s="15"/>
       <c r="K19" s="15">
         <f>K21/2</f>
-        <v>1.4018958157520383</v>
+        <v>2.2312263051883439</v>
       </c>
       <c r="L19" s="15"/>
     </row>
@@ -1803,7 +1831,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -1812,7 +1840,7 @@
       <c r="H21" s="15"/>
       <c r="K21" s="15">
         <f>SQRT(4*K17/3.14159)</f>
-        <v>2.8037916315040765</v>
+        <v>4.4624526103766877</v>
       </c>
       <c r="L21" s="15"/>
     </row>
@@ -1821,7 +1849,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -1836,10 +1864,10 @@
     </row>
     <row r="25" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
@@ -1848,16 +1876,16 @@
       <c r="H25" s="15"/>
       <c r="K25" s="15">
         <f>0.382*K3</f>
-        <v>0.23955433215310007</v>
+        <v>0.38126936496710612</v>
       </c>
       <c r="L25" s="15"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>56</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -1866,16 +1894,16 @@
       <c r="H27" s="15"/>
       <c r="K27" s="15">
         <f>1.5*K3</f>
-        <v>0.94065837232892702</v>
+        <v>1.4971310142687413</v>
       </c>
       <c r="L27" s="15"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>62</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>65</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
@@ -1884,13 +1912,13 @@
       <c r="H32" s="15"/>
       <c r="K32" s="15">
         <f>(K13-K3)/TAN(RADIANS(K36))*K34</f>
-        <v>1.7047349748173977</v>
+        <v>2.7132183978641256</v>
       </c>
       <c r="L32" s="15"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" s="15">
         <v>0.8</v>
@@ -1907,7 +1935,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C36" s="15">
         <v>15</v>
@@ -1924,10 +1952,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
@@ -1936,16 +1964,16 @@
       <c r="H38" s="15"/>
       <c r="K38" s="15">
         <f>(K5/2)*SIN(RADIANS(K3-90+180))/SIN(RADIANS(K3))</f>
-        <v>57.293491592666015</v>
+        <v>57.289983865154419</v>
       </c>
       <c r="L38" s="15"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
@@ -1954,7 +1982,7 @@
       <c r="H40" s="15"/>
       <c r="K40" s="15">
         <f>K11/2*SIN(K36-90+180)/SIN(K36)</f>
-        <v>-1.7881040793985641</v>
+        <v>-2.8459068167119344</v>
       </c>
       <c r="L40" s="15"/>
     </row>

</xml_diff>

<commit_message>
some changes - design docs
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F04533-3788-5640-ABF6-85D243FE2B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509DAF20-3FC9-ED43-B25D-2EDE2F97F154}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="500" windowWidth="14280" windowHeight="16280" activeTab="1" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="12440" yWindow="500" windowWidth="17760" windowHeight="16280" activeTab="2" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Geometry" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>M = Gas Molecular Weight (Combustion of gaseous/hydrocarbon fuel)  = 24</t>
   </si>
@@ -332,6 +331,9 @@
   </si>
   <si>
     <t>sqrt(2 / (gamma - 1) * ((pc / pa) ** ((gamma - 1) / gamma) - 1))</t>
+  </si>
+  <si>
+    <t>pressure:kpa</t>
   </si>
 </sst>
 </file>
@@ -453,14 +455,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D768E0CB-7D5E-604F-9A57-088686C5C71F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,6 +991,11 @@
         <v>78</v>
       </c>
       <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -999,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D17"/>
+    <sheetView topLeftCell="E3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1285,25 +1292,25 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="C27:H27"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="K21:L21"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B15:D15"/>
     <mergeCell ref="C29:H29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="C22:H22"/>
     <mergeCell ref="C23:H23"/>
     <mergeCell ref="K23:L23"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="K25:L25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1314,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,7 +1333,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>79</v>
       </c>
       <c r="B1" s="15"/>
@@ -1336,14 +1343,14 @@
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="K2" s="17" t="s">
+      <c r="F2" s="16"/>
+      <c r="K2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="17"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1515,23 +1522,23 @@
       <c r="A20" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="K20" s="16">
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="K20" s="18">
         <v>263.38618498858511</v>
       </c>
-      <c r="L20" s="16"/>
+      <c r="L20" s="18"/>
       <c r="M20" s="14">
         <f>SQRT(Constants!K29*Constants!K25*Constants!B11)/Constants!K25*SQRT(POWER(2/Constants!K25+1,Constants!K25+1/Constants!K25-1))</f>
         <v>263.38618498858511</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N20" s="18">
         <v>2.5982911572999998</v>
       </c>
       <c r="O20" s="15"/>
@@ -1540,12 +1547,12 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1602,16 +1609,22 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K6:L6"/>
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C4:H4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K6:L6"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="K25:L25"/>
@@ -1623,12 +1636,6 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="C20:H21"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1640,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A288A652-25F1-A940-BC3C-A6B5AB550EFC}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1988,6 +1995,30 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C23:H23"/>
     <mergeCell ref="C38:H38"/>
     <mergeCell ref="C40:H40"/>
     <mergeCell ref="K38:L38"/>
@@ -2000,30 +2031,6 @@
     <mergeCell ref="K34:L34"/>
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new documentation for sbc power config and other changes
</commit_message>
<xml_diff>
--- a/Nozzle-CC/Converse Engine v1.xlsx
+++ b/Nozzle-CC/Converse Engine v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Nozzle-CC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A56F6A8-CB87-F646-9482-7002C7805037}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F632289-A4F5-B943-BF79-EE9D0A882601}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="2" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{6B94F6F9-44B0-CC46-BCE3-E21706DCCC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="4" r:id="rId1"/>
@@ -327,13 +327,13 @@
     <t>pressure:kpa</t>
   </si>
   <si>
-    <t>(1.1)*Chamber Area * Chamber Length</t>
-  </si>
-  <si>
     <t>50 atm</t>
   </si>
   <si>
     <t>Expansion ratio * Throat Area</t>
+  </si>
+  <si>
+    <t>Throat Area * Chamber characteristic length</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0A97E6-915A-D143-A6DF-A3F09B431841}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K20" sqref="K20:L20"/>
     </sheetView>
   </sheetViews>
@@ -1116,7 +1116,7 @@
         <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1320,7 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D475DE-CC2C-7C4E-9119-639F39D169A8}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="L2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:H6"/>
     </sheetView>
   </sheetViews>
@@ -1649,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A288A652-25F1-A940-BC3C-A6B5AB550EFC}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="92" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1722,7 +1722,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -1786,7 +1786,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -1794,7 +1794,7 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="K15" s="15">
-        <f ca="1">(1.1)*K17*K23</f>
+        <f>K7*Properties!K18</f>
         <v>0</v>
       </c>
       <c r="L15" s="15"/>
@@ -1865,9 +1865,9 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="K23" s="15" t="e">
-        <f ca="1">K15/(1.1*K17)</f>
-        <v>#VALUE!</v>
+      <c r="K23" s="15">
+        <f>K15/(1.1*K17)</f>
+        <v>0</v>
       </c>
       <c r="L23" s="15"/>
     </row>

</xml_diff>